<commit_message>
limitado ao ano de publicacao
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Artigos_Completos.xlsx
+++ b/Experiment01_Resumo/Resumo_Artigos_Completos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -1333,96 +1333,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1439,111 +1352,198 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1828,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,22 +1839,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="54"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
@@ -1897,12 +1897,12 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="B9" s="38"/>
-    </row>
-    <row r="10" spans="1:2" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+    </row>
+    <row r="10" spans="1:2" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>204</v>
       </c>
@@ -1934,8 +1934,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
+    <row r="14" spans="1:2" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
         <v>201</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -1951,8 +1951,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="66"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1975,211 +1975,211 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="39" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="71"/>
     </row>
     <row r="2" spans="1:12" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="62"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="45"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="62"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="65"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="65"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="48"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="68"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="62"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="45"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="45"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="65"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="48"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="33" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2188,47 +2188,47 @@
       <c r="A18" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="74"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="73"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="79"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="53"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="75"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="79"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="53"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="75"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80"/>
@@ -2246,16 +2246,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L5"/>
+    <mergeCell ref="B6:L9"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="B18:L21"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B10:L13"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L5"/>
-    <mergeCell ref="B6:L9"/>
-    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2266,36 +2266,36 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="64" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="35" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2314,67 +2314,67 @@
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="65"/>
-      <c r="E4" s="67" t="s">
+      <c r="C4" s="36"/>
+      <c r="E4" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="99" t="s">
+      <c r="J4" s="109" t="s">
         <v>212</v>
       </c>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="10">
@@ -2383,24 +2383,24 @@
       <c r="I5" s="10">
         <v>17</v>
       </c>
-      <c r="J5" s="100" t="s">
+      <c r="J5" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
     </row>
     <row r="6" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="10">
@@ -2409,27 +2409,27 @@
       <c r="I6" s="10">
         <v>10</v>
       </c>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
     </row>
     <row r="7" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
       <c r="E7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H7" s="10">
@@ -2438,25 +2438,25 @@
       <c r="I7" s="10">
         <v>16</v>
       </c>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="97"/>
-      <c r="C8" s="54"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
       <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H8" s="10">
@@ -2465,48 +2465,48 @@
       <c r="I8" s="10">
         <v>103</v>
       </c>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
-      <c r="O8" s="100"/>
-      <c r="P8" s="100"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="108"/>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="104"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="54"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="103"/>
       <c r="E9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="65"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="10">
         <v>43</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="100"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="104"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="54"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="103"/>
       <c r="E10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="10">
@@ -2515,25 +2515,25 @@
       <c r="I10" s="10">
         <v>128</v>
       </c>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="100"/>
-      <c r="P10" s="100"/>
+      <c r="J10" s="108"/>
+      <c r="K10" s="108"/>
+      <c r="L10" s="108"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="108"/>
+      <c r="O10" s="108"/>
+      <c r="P10" s="108"/>
     </row>
     <row r="11" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="106"/>
       <c r="E11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="36" t="s">
         <v>36</v>
       </c>
       <c r="H11" s="10">
@@ -2542,16 +2542,16 @@
       <c r="I11" s="10">
         <v>182</v>
       </c>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
+      <c r="J11" s="108"/>
+      <c r="K11" s="108"/>
+      <c r="L11" s="108"/>
+      <c r="M11" s="108"/>
+      <c r="N11" s="108"/>
+      <c r="O11" s="108"/>
+      <c r="P11" s="108"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="40"/>
       <c r="G12" t="s">
         <v>138</v>
       </c>
@@ -2565,156 +2565,156 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="40"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="69"/>
+      <c r="B14" s="40"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="B15" s="90"/>
-      <c r="C15" s="91"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="93"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="45"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="92" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="93"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="93"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="93"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="93"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="92" t="s">
+      <c r="A21" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="93"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="93"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
+      <c r="A24" s="35"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
     </row>
     <row r="26" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="84"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="89"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="84"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="89"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="84"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="89"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="87"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="97"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="84"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="89"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="89"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="83"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="84"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="89"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2728,12 +2728,12 @@
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2743,15 +2743,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="24"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
@@ -2761,52 +2761,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="110" t="s">
+      <c r="F2" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="110" t="s">
+      <c r="H2" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="I2" s="110" t="s">
+      <c r="I2" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="J2" s="110" t="s">
+      <c r="J2" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="K2" s="111" t="s">
+      <c r="K2" s="50" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3543,6 +3543,10 @@
       <c r="I25" s="25">
         <f>SUM(I3:I24)</f>
         <v>515</v>
+      </c>
+      <c r="J25" s="12">
+        <f>SUM(J3:J24)</f>
+        <v>541</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.25">

</xml_diff>